<commit_message>
findContainerClass.R is a new helper file that helps isolate the correct container whichhas been a frequent problem with the code All other changes are largerly incremental The other updated file is the ErrorTracking worksheet which has been updated with the successful debugs This needs to be regenerated. so that we can make sure that the changes we are making aren't having a negative effect on othes
</commit_message>
<xml_diff>
--- a/tracking/ErrorTrackingWorksheet.xlsx
+++ b/tracking/ErrorTrackingWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExecutiveSearchYaml\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EA1A04-9699-41E8-9387-DFB1FF8E6566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2D7D3C-8242-4DDF-99E4-3E4F5D90633B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{9D0ED3D9-8DC4-4D4C-858D-9FAFB5864947}"/>
+    <workbookView xWindow="18850" yWindow="2410" windowWidth="16710" windowHeight="17860" activeTab="1" xr2:uid="{9D0ED3D9-8DC4-4D4C-858D-9FAFB5864947}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="180">
   <si>
     <t>WRHN-KITCHENER ST MARY'S</t>
   </si>
@@ -573,37 +573,10 @@
     <t>rowid</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>Dr. Simon O’Brien</t>
-  </si>
-  <si>
-    <t>Joanne simons</t>
-  </si>
-  <si>
-    <t>Sanaz Riahi</t>
-  </si>
-  <si>
-    <t>Dr. Anne-Claude Gingras</t>
-  </si>
-  <si>
-    <t>missing 2</t>
-  </si>
-  <si>
-    <t>Fails</t>
-  </si>
-  <si>
-    <t>fails</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Fixed</t>
+    <t>Robotxt</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -2181,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90A319D-8BC4-42E9-A83E-FF2B7638B895}">
   <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3138,7 +3111,7 @@
         <v>3</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>179</v>
+        <v>2</v>
       </c>
       <c r="I33" s="7">
         <v>-12</v>
@@ -3167,7 +3140,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>179</v>
+        <v>2</v>
       </c>
       <c r="I34" s="7">
         <v>-12</v>
@@ -3196,7 +3169,7 @@
         <v>3</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>179</v>
+        <v>2</v>
       </c>
       <c r="I35" s="7">
         <v>-12</v>
@@ -3602,7 +3575,7 @@
         <v>12</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>180</v>
+        <v>2</v>
       </c>
       <c r="I49" s="7">
         <v>1</v>
@@ -3660,7 +3633,7 @@
         <v>6</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>181</v>
+        <v>2</v>
       </c>
       <c r="I51" s="7">
         <v>1</v>
@@ -3689,7 +3662,7 @@
         <v>6</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>182</v>
+        <v>2</v>
       </c>
       <c r="I52" s="7">
         <v>1</v>
@@ -3718,7 +3691,7 @@
         <v>16</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>183</v>
+        <v>2</v>
       </c>
       <c r="I53" s="7">
         <v>1</v>
@@ -3747,7 +3720,7 @@
         <v>11</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>184</v>
+        <v>2</v>
       </c>
       <c r="I54" s="7">
         <v>2</v>
@@ -3776,7 +3749,7 @@
         <v>5</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
       <c r="I55" s="7">
         <v>4</v>
@@ -3863,7 +3836,7 @@
         <v>14</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
       <c r="I58" s="7">
         <v>13</v>
@@ -3892,7 +3865,7 @@
         <v>15</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="I59" s="7">
         <v>14</v>
@@ -3921,7 +3894,7 @@
         <v>17</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I60" s="7">
         <v>16</v>

</xml_diff>